<commit_message>
feat: download file done
</commit_message>
<xml_diff>
--- a/src/files/archivo_actualizado_ciael.xlsx
+++ b/src/files/archivo_actualizado_ciael.xlsx
@@ -363,30 +363,69 @@
     <t>Cerrado</t>
   </si>
   <si>
+    <t xml:space="preserve">dfhgfhfghgfhgfh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AGUILAR CAMACHO YURITZY AMEYALIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Femenino</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2003-04-19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-10-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OCTUBRE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Atrapamiento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jefe de Servicios Generales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diurna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-01-06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hidrogeno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Muestreo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alejandro Lazcano</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Físico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Charet Macias</t>
+  </si>
+  <si>
     <t xml:space="preserve">Completo</t>
   </si>
   <si>
     <t xml:space="preserve">OLGUIN CRUZ BRENDA</t>
   </si>
   <si>
-    <t xml:space="preserve">Femenino</t>
-  </si>
-  <si>
     <t xml:space="preserve">1996-03-08</t>
   </si>
   <si>
     <t xml:space="preserve">2025-10-01</t>
   </si>
   <si>
-    <t xml:space="preserve">OCTUBRE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Atrapamiento</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CCM</t>
-  </si>
-  <si>
     <t xml:space="preserve">Operador ayudante de mezclado</t>
   </si>
   <si>
@@ -396,9 +435,6 @@
     <t xml:space="preserve">Caída de objetos</t>
   </si>
   <si>
-    <t xml:space="preserve">Diurna</t>
-  </si>
-  <si>
     <t xml:space="preserve">2025-03-25</t>
   </si>
   <si>
@@ -408,12 +444,6 @@
     <t xml:space="preserve">Sacheteadora</t>
   </si>
   <si>
-    <t xml:space="preserve">Muestreo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alejandro Lazcano</t>
-  </si>
-  <si>
     <t xml:space="preserve">Condiciones de seguridad</t>
   </si>
   <si>
@@ -429,13 +459,7 @@
     <t xml:space="preserve"/>
   </si>
   <si>
-    <t xml:space="preserve">2025-10-10</t>
-  </si>
-  <si>
     <t xml:space="preserve">Maceraciones</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SI</t>
   </si>
   <si>
     <t xml:space="preserve">Erika Sanchez</t>
@@ -2487,7 +2511,7 @@
         <v>94</v>
       </c>
       <c r="C9" s="12">
-        <v>20159</v>
+        <v>10827</v>
       </c>
       <c r="D9" t="s" s="13">
         <v>95</v>
@@ -2499,7 +2523,7 @@
         <v>97</v>
       </c>
       <c r="G9" s="15">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="H9" t="s" s="14">
         <v>98</v>
@@ -2514,7 +2538,7 @@
         <v>100</v>
       </c>
       <c r="L9" s="12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M9" t="s" s="17">
         <v>101</v>
@@ -2523,61 +2547,61 @@
         <v>102</v>
       </c>
       <c r="O9" t="s" s="17">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="P9" t="s" s="11">
-        <v>103</v>
+        <v>43</v>
       </c>
       <c r="Q9" t="s" s="11">
         <v>36</v>
       </c>
       <c r="R9" t="s" s="11">
-        <v>104</v>
+        <v>57</v>
       </c>
       <c r="S9" t="s" s="12">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="T9" s="12">
         <v>2</v>
       </c>
       <c r="U9" t="s" s="14">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="V9" t="s" s="12">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="W9" t="s" s="12">
         <v>39</v>
       </c>
       <c r="X9" t="s" s="12">
+        <v>105</v>
+      </c>
+      <c r="Y9" t="s" s="17">
+        <v>106</v>
+      </c>
+      <c r="Z9" t="s" s="12">
+        <v>105</v>
+      </c>
+      <c r="AA9" s="15">
+        <v>9</v>
+      </c>
+      <c r="AB9" t="s" s="13">
         <v>107</v>
-      </c>
-      <c r="Y9" t="s" s="17">
-        <v>108</v>
-      </c>
-      <c r="Z9" t="s" s="12">
-        <v>107</v>
-      </c>
-      <c r="AA9" s="15">
-        <v>7</v>
-      </c>
-      <c r="AB9" t="s" s="13">
-        <v>109</v>
       </c>
       <c r="AC9" t="s" s="12">
         <v>101</v>
       </c>
       <c r="AD9" t="s" s="12">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="AE9" t="s" s="12">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="AF9" t="s" s="12">
         <v>52</v>
       </c>
       <c r="AG9" t="s" s="12">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:33">
@@ -2585,25 +2609,25 @@
         <v>63</v>
       </c>
       <c r="B10" t="s" s="11">
+        <v>111</v>
+      </c>
+      <c r="C10" s="12">
+        <v>20159</v>
+      </c>
+      <c r="D10" t="s" s="13">
+        <v>112</v>
+      </c>
+      <c r="E10" t="s" s="12">
+        <v>96</v>
+      </c>
+      <c r="F10" t="s" s="14">
         <v>113</v>
       </c>
-      <c r="C10" s="12">
-        <v>10877</v>
-      </c>
-      <c r="D10" t="s" s="13">
+      <c r="G10" s="15">
+        <v>29</v>
+      </c>
+      <c r="H10" t="s" s="14">
         <v>114</v>
-      </c>
-      <c r="E10" t="s" s="12">
-        <v>115</v>
-      </c>
-      <c r="F10" t="s" s="14">
-        <v>115</v>
-      </c>
-      <c r="G10" t="s" s="15">
-        <v>115</v>
-      </c>
-      <c r="H10" t="s" s="14">
-        <v>116</v>
       </c>
       <c r="I10" s="12">
         <v>2025</v>
@@ -2614,101 +2638,167 @@
       <c r="K10" t="s" s="16">
         <v>100</v>
       </c>
-      <c r="L10" s="12"/>
+      <c r="L10" s="12">
+        <v>3</v>
+      </c>
       <c r="M10" t="s" s="17">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="N10" t="s" s="11">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="O10" t="s" s="17">
         <v>64</v>
       </c>
       <c r="P10" t="s" s="11">
+        <v>116</v>
+      </c>
+      <c r="Q10" t="s" s="11">
+        <v>36</v>
+      </c>
+      <c r="R10" t="s" s="11">
+        <v>117</v>
+      </c>
+      <c r="S10" t="s" s="12">
         <v>103</v>
       </c>
-      <c r="Q10" t="s" s="11">
-        <v>70</v>
-      </c>
-      <c r="R10" t="s" s="11">
-        <v>65</v>
-      </c>
-      <c r="S10" t="s" s="12">
-        <v>105</v>
-      </c>
       <c r="T10" s="12">
-        <v>1</v>
-      </c>
-      <c r="U10" s="14"/>
+        <v>2</v>
+      </c>
+      <c r="U10" t="s" s="14">
+        <v>118</v>
+      </c>
       <c r="V10" t="s" s="12">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="W10" t="s" s="12">
         <v>39</v>
       </c>
       <c r="X10" t="s" s="12">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="Y10" t="s" s="17">
+        <v>120</v>
+      </c>
+      <c r="Z10" t="s" s="12">
+        <v>119</v>
+      </c>
+      <c r="AA10" s="15">
+        <v>7</v>
+      </c>
+      <c r="AB10" t="s" s="13">
+        <v>107</v>
+      </c>
+      <c r="AC10" t="s" s="12">
+        <v>101</v>
+      </c>
+      <c r="AD10" t="s" s="12">
         <v>108</v>
       </c>
-      <c r="Z10" t="s" s="12">
-        <v>118</v>
-      </c>
-      <c r="AA10" s="15"/>
-      <c r="AB10" t="s" s="13">
-        <v>109</v>
-      </c>
-      <c r="AC10" t="s" s="12">
-        <v>117</v>
-      </c>
-      <c r="AD10" t="s" s="12">
-        <v>119</v>
-      </c>
       <c r="AE10" t="s" s="12">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="AF10" t="s" s="12">
         <v>52</v>
       </c>
       <c r="AG10" t="s" s="12">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33">
+      <c r="A11" t="s" s="10">
+        <v>63</v>
+      </c>
+      <c r="B11" t="s" s="11">
+        <v>123</v>
+      </c>
+      <c r="C11" s="12">
+        <v>10877</v>
+      </c>
+      <c r="D11" t="s" s="13">
+        <v>124</v>
+      </c>
+      <c r="E11" t="s" s="12">
+        <v>125</v>
+      </c>
+      <c r="F11" t="s" s="14">
+        <v>125</v>
+      </c>
+      <c r="G11" t="s" s="15">
+        <v>125</v>
+      </c>
+      <c r="H11" t="s" s="14">
+        <v>98</v>
+      </c>
+      <c r="I11" s="12">
+        <v>2025</v>
+      </c>
+      <c r="J11" t="s" s="12">
+        <v>99</v>
+      </c>
+      <c r="K11" t="s" s="16">
+        <v>100</v>
+      </c>
+      <c r="L11" s="12"/>
+      <c r="M11" t="s" s="17">
+        <v>126</v>
+      </c>
+      <c r="N11" t="s" s="11">
         <v>115</v>
       </c>
-    </row>
-    <row r="11" spans="1:33">
-      <c r="A11" s="10"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="16"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="17"/>
-      <c r="N11" s="11"/>
-      <c r="O11" s="17"/>
-      <c r="P11" s="11"/>
-      <c r="Q11" s="11"/>
-      <c r="R11" s="11"/>
-      <c r="S11" s="12"/>
-      <c r="T11" s="12"/>
+      <c r="O11" t="s" s="17">
+        <v>64</v>
+      </c>
+      <c r="P11" t="s" s="11">
+        <v>116</v>
+      </c>
+      <c r="Q11" t="s" s="11">
+        <v>70</v>
+      </c>
+      <c r="R11" t="s" s="11">
+        <v>65</v>
+      </c>
+      <c r="S11" t="s" s="12">
+        <v>103</v>
+      </c>
+      <c r="T11" s="12">
+        <v>1</v>
+      </c>
       <c r="U11" s="14"/>
-      <c r="V11" s="12"/>
-      <c r="W11" s="12"/>
-      <c r="X11" s="12"/>
-      <c r="Y11" s="17"/>
-      <c r="Z11" s="12"/>
+      <c r="V11" t="s" s="12">
+        <v>105</v>
+      </c>
+      <c r="W11" t="s" s="12">
+        <v>39</v>
+      </c>
+      <c r="X11" t="s" s="12">
+        <v>105</v>
+      </c>
+      <c r="Y11" t="s" s="17">
+        <v>120</v>
+      </c>
+      <c r="Z11" t="s" s="12">
+        <v>105</v>
+      </c>
       <c r="AA11" s="15"/>
-      <c r="AB11" s="13"/>
-      <c r="AC11" s="12"/>
-      <c r="AD11" s="12"/>
-      <c r="AE11" s="12"/>
-      <c r="AF11" s="12"/>
-      <c r="AG11" s="12"/>
+      <c r="AB11" t="s" s="13">
+        <v>107</v>
+      </c>
+      <c r="AC11" t="s" s="12">
+        <v>126</v>
+      </c>
+      <c r="AD11" t="s" s="12">
+        <v>127</v>
+      </c>
+      <c r="AE11" t="s" s="12">
+        <v>128</v>
+      </c>
+      <c r="AF11" t="s" s="12">
+        <v>52</v>
+      </c>
+      <c r="AG11" t="s" s="12">
+        <v>125</v>
+      </c>
     </row>
     <row r="12" spans="1:33">
       <c r="A12" s="10"/>

</xml_diff>